<commit_message>
Added Linear Regression for Circular and updated database and correlation code
</commit_message>
<xml_diff>
--- a/Database/SS CFST Database_Finalised_for correlation.xlsx
+++ b/Database/SS CFST Database_Finalised_for correlation.xlsx
@@ -37,7 +37,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhFgRjDNxtBdiXGcJjsZKhNDdFLiQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhVw87y0ouvH8koiVoZ3gG9Qu9umg=="/>
     </ext>
   </extLst>
 </comments>
@@ -63,7 +63,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJcWB7B/iDynyTWrhF8KUoWsWsgg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgHM63IFUvjBejjOUr+oYvtQttY6g=="/>
     </ext>
   </extLst>
 </comments>
@@ -368,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -425,6 +425,9 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -48270,7 +48273,9 @@
       <c r="G179" s="19">
         <v>562.1</v>
       </c>
-      <c r="H179" s="20"/>
+      <c r="H179" s="21">
+        <v>8.3</v>
+      </c>
       <c r="I179" s="19">
         <v>35.8</v>
       </c>
@@ -48300,7 +48305,9 @@
       <c r="G180" s="19">
         <v>656.4</v>
       </c>
-      <c r="H180" s="20"/>
+      <c r="H180" s="21">
+        <v>8.3</v>
+      </c>
       <c r="I180" s="19">
         <v>35.8</v>
       </c>
@@ -48330,7 +48337,9 @@
       <c r="G181" s="19">
         <v>617.8</v>
       </c>
-      <c r="H181" s="20"/>
+      <c r="H181" s="21">
+        <v>8.3</v>
+      </c>
       <c r="I181" s="19">
         <v>35.8</v>
       </c>

</xml_diff>